<commit_message>
automation framework - excelutils
</commit_message>
<xml_diff>
--- a/AutomationFramework/testdata/OpenEmrTestData.xlsx
+++ b/AutomationFramework/testdata/OpenEmrTestData.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="1" r:id="rId1"/>
-    <sheet name="patientErrorMessageTest" sheetId="2" r:id="rId2"/>
+    <sheet name="invalidCredentialTestCount" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
   <si>
     <t>Password</t>
   </si>
@@ -36,9 +36,6 @@
     <t>ExpectedValue</t>
   </si>
   <si>
-    <t>john</t>
-  </si>
-  <si>
     <t>john123</t>
   </si>
   <si>
@@ -58,6 +55,18 @@
   </si>
   <si>
     <t>Username</t>
+  </si>
+  <si>
+    <t>bala</t>
+  </si>
+  <si>
+    <t>Rows to be tested</t>
+  </si>
+  <si>
+    <t>paul</t>
+  </si>
+  <si>
+    <t>mark</t>
   </si>
 </sst>
 </file>
@@ -377,8 +386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,7 +400,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -405,30 +414,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -438,12 +447,99 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
automation framework - final
</commit_message>
<xml_diff>
--- a/AutomationFramework/testdata/OpenEmrTestData.xlsx
+++ b/AutomationFramework/testdata/OpenEmrTestData.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="1" r:id="rId1"/>
     <sheet name="invalidCredentialTestCount" sheetId="2" r:id="rId2"/>
+    <sheet name="patientErrorMessageTest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>Password</t>
   </si>
@@ -67,6 +68,36 @@
   </si>
   <si>
     <t>mark</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>User Id</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>English (Indian)</t>
+  </si>
+  <si>
+    <t>Please book an appointment</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Please choose a patient</t>
+  </si>
+  <si>
+    <t>accountant</t>
   </si>
 </sst>
 </file>
@@ -387,7 +418,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -542,4 +573,95 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>